<commit_message>
Fixed overwrite bug in excel
</commit_message>
<xml_diff>
--- a/dataGen/stego_training.xlsx
+++ b/dataGen/stego_training.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B1" t="b">
@@ -434,11 +434,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_house_0.jpg</t>
         </is>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -454,11 +454,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_falls_1.jpg</t>
         </is>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -474,17 +474,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_boat_2.jpg</t>
         </is>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B7" t="b">
@@ -494,11 +494,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_girl_3.jpg</t>
         </is>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -514,11 +514,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_girl_4.jpg</t>
         </is>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -534,17 +534,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_house_5.jpg</t>
         </is>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B13" t="b">
@@ -554,17 +554,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_house_6.jpg</t>
         </is>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
         </is>
       </c>
       <c r="B15" t="b">
@@ -574,17 +574,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_boat_7.jpg</t>
         </is>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
         </is>
       </c>
       <c r="B17" t="b">
@@ -594,11 +594,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_boat_8.jpg</t>
         </is>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -614,17 +614,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_boat_9.jpg</t>
         </is>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B21" t="b">
@@ -634,11 +634,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_girl_10.jpg</t>
         </is>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -654,11 +654,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_boat_11.jpg</t>
         </is>
       </c>
       <c r="B24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -674,11 +674,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_falls_12.jpg</t>
         </is>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -694,17 +694,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_house_13.jpg</t>
         </is>
       </c>
       <c r="B28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B29" t="b">
@@ -714,17 +714,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_girl_14.jpg</t>
         </is>
       </c>
       <c r="B30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B31" t="b">
@@ -734,17 +734,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_house_15.jpg</t>
         </is>
       </c>
       <c r="B32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B33" t="b">
@@ -754,17 +754,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_girl_16.jpg</t>
         </is>
       </c>
       <c r="B34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B35" t="b">
@@ -774,17 +774,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_girl_17.jpg</t>
         </is>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
         </is>
       </c>
       <c r="B37" t="b">
@@ -794,17 +794,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_18.jpg</t>
         </is>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
         </is>
       </c>
       <c r="B39" t="b">
@@ -814,11 +814,11 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_boat_19.jpg</t>
         </is>
       </c>
       <c r="B40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -834,17 +834,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_girl_20.jpg</t>
         </is>
       </c>
       <c r="B42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B43" t="b">
@@ -854,11 +854,11 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_house_21.jpg</t>
         </is>
       </c>
       <c r="B44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -874,17 +874,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_falls_22.jpg</t>
         </is>
       </c>
       <c r="B46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B47" t="b">
@@ -894,17 +894,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_house_23.jpg</t>
         </is>
       </c>
       <c r="B48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
         </is>
       </c>
       <c r="B49" t="b">
@@ -914,20 +914,510 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_house_24.jpg</t>
         </is>
       </c>
       <c r="B50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_boat_49.jpg</t>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
         </is>
       </c>
       <c r="B51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_falls_25.jpg</t>
+        </is>
+      </c>
+      <c r="B52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_26.jpg</t>
+        </is>
+      </c>
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+        </is>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_house_27.jpg</t>
+        </is>
+      </c>
+      <c r="B56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_boat_28.jpg</t>
+        </is>
+      </c>
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_boat_29.jpg</t>
+        </is>
+      </c>
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_girl_30.jpg</t>
+        </is>
+      </c>
+      <c r="B62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_girl_31.jpg</t>
+        </is>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_girl_32.jpg</t>
+        </is>
+      </c>
+      <c r="B66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_girl_33.jpg</t>
+        </is>
+      </c>
+      <c r="B68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+        </is>
+      </c>
+      <c r="B69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_house_34.jpg</t>
+        </is>
+      </c>
+      <c r="B70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+        </is>
+      </c>
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_house_35.jpg</t>
+        </is>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_secret_cover_boat_36.jpg</t>
+        </is>
+      </c>
+      <c r="B74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_boat_37.jpg</t>
+        </is>
+      </c>
+      <c r="B76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_boat_38.jpg</t>
+        </is>
+      </c>
+      <c r="B78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_girl_39.jpg</t>
+        </is>
+      </c>
+      <c r="B80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+        </is>
+      </c>
+      <c r="B81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_falls_40.jpg</t>
+        </is>
+      </c>
+      <c r="B82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_house.jpg</t>
+        </is>
+      </c>
+      <c r="B83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_house_41.jpg</t>
+        </is>
+      </c>
+      <c r="B84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_42.jpg</t>
+        </is>
+      </c>
+      <c r="B86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_43.jpg</t>
+        </is>
+      </c>
+      <c r="B88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/joly_beans,_holy_greens,_and_billy_jeen_cover_boat_44.jpg</t>
+        </is>
+      </c>
+      <c r="B90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_45.jpg</t>
+        </is>
+      </c>
+      <c r="B92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_boat.jpg</t>
+        </is>
+      </c>
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_boat_46.jpg</t>
+        </is>
+      </c>
+      <c r="B94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+        </is>
+      </c>
+      <c r="B95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_falls_47.jpg</t>
+        </is>
+      </c>
+      <c r="B96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_falls.jpg</t>
+        </is>
+      </c>
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/woah_oh_ohhhhhh_cover_falls_48.jpg</t>
+        </is>
+      </c>
+      <c r="B98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/cover_girl.jpg</t>
+        </is>
+      </c>
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>/home/kdaus/Anti_Forensic_Deep_Learning_Tool/dataGen/gen_data/My_super_duper_secret_cover_girl_49.jpg</t>
+        </is>
+      </c>
+      <c r="B100" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>